<commit_message>
Changes made in formul excel file
</commit_message>
<xml_diff>
--- a/Formula Excel Template.xlsx
+++ b/Formula Excel Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sadiqunnurayan/Documents/GitHub/Excel-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492A496C-BD30-4402-B2BA-8A5A15968915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAE6F77-1510-4A47-946D-85AF89D7DF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" firstSheet="1" activeTab="7" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Max-Min" sheetId="9" r:id="rId1"/>
@@ -372,11 +372,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,13 +699,13 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -741,7 +740,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -769,16 +768,16 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2">
         <f>MAX(G2:G10)</f>
         <v>65000</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2">
         <f>MIN(G2:G10)</f>
         <v>36000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -807,7 +806,7 @@
         <v>42287</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -836,7 +835,7 @@
         <v>42986</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -865,7 +864,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -894,7 +893,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -923,7 +922,7 @@
         <v>41528</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -952,7 +951,7 @@
         <v>41551</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -981,7 +980,7 @@
         <v>42116</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1026,17 +1025,17 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1108,7 +1107,7 @@
         <v>Jim.Halpert@gmail.com</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>Pam.Beasley@gmail.com</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>Dwight.Schrute@gmail.com</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>Angela.Martin@gmail.com</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>Toby.Flenderson@gmail.com</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>Michael.Scott@gmail.com</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1330,7 +1329,7 @@
         <v>Meredith.Palmer@gmail.com</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>Stanley.Hudson@gmail.com</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1404,13 +1403,13 @@
         <v>Kevin.Malone@gmail.com</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H11" t="str">
         <f t="shared" ref="H11:H12" si="2">CONCATENATE(B11," ",C11)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H12" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
@@ -1432,13 +1431,13 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1502,7 +1501,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1560,7 +1559,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1589,7 +1588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1647,7 +1646,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1676,7 +1675,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1745,7 +1744,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1758,18 +1757,18 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1804,7 +1803,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>Salesman</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1876,7 +1875,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>Salesman</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1946,7 +1945,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1981,7 +1980,7 @@
         <v>HR</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -2016,7 +2015,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>Salesman</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -2137,12 +2136,12 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2177,7 +2176,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -2242,7 +2241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -2274,7 +2273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -2338,7 +2337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -2370,7 +2369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -2482,13 +2481,13 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="10" max="10" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2529,7 +2528,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -2573,7 +2572,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -2655,7 +2654,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -2696,7 +2695,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -2737,7 +2736,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -2778,7 +2777,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -2860,7 +2859,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -2917,13 +2916,13 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2955,7 +2954,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -2997,7 +2996,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3075,7 +3074,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3114,7 +3113,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3192,7 +3191,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3231,7 +3230,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -3309,10 +3308,10 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H13" s="2"/>
     </row>
   </sheetData>
@@ -3331,13 +3330,13 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3372,7 +3371,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>Halpert</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3437,7 +3436,7 @@
         <v>Beasley</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3469,7 +3468,7 @@
         <v>Schrute</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>Martin</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3533,7 +3532,7 @@
         <v>Flenderson</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3565,7 +3564,7 @@
         <v>Scott</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3597,7 +3596,7 @@
         <v>Palmer</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -3629,7 +3628,7 @@
         <v>Hudson</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -3677,13 +3676,13 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3721,7 +3720,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -3762,7 +3761,7 @@
         <v>11/2/2001</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3800,7 +3799,7 @@
         <v>10/3/1999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3838,7 +3837,7 @@
         <v>7/4/2000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3876,7 +3875,7 @@
         <v>1/5/2000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3914,7 +3913,7 @@
         <v>5/6/2001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>5/6/2001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3990,7 +3989,7 @@
         <v>11/8/2003</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -4028,7 +4027,7 @@
         <v>6/9/2002</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -4066,39 +4065,39 @@
         <v>8/10/2003</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
@@ -4115,13 +4114,13 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -4200,7 +4199,7 @@
         <v>88000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -4229,7 +4228,7 @@
         <v>42287</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -4258,7 +4257,7 @@
         <v>42986</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -4345,7 +4344,7 @@
         <v>41528</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -4374,7 +4373,7 @@
         <v>41551</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -4403,7 +4402,7 @@
         <v>42116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -4448,13 +4447,13 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -4492,7 +4491,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -4521,7 +4520,7 @@
         <v>42253</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -4550,7 +4549,7 @@
         <v>42287</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -4579,7 +4578,7 @@
         <v>42986</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -4608,7 +4607,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -4637,7 +4636,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>41528</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -4695,7 +4694,7 @@
         <v>41551</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -4724,7 +4723,7 @@
         <v>42116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>

</xml_diff>